<commit_message>
added the new worksheet
</commit_message>
<xml_diff>
--- a/Collected_Data_Result.xlsx
+++ b/Collected_Data_Result.xlsx
@@ -5,15 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x012180\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X007944\Desktop\T-factors\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Collected_Data" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collected_Data!$A$1:$I$138</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="127">
   <si>
     <t>Emp Id</t>
   </si>
@@ -128,12 +131,6 @@
     <t>Jagrut Sachdev</t>
   </si>
   <si>
-    <t>Self-242168</t>
-  </si>
-  <si>
-    <t>The Table doesn't contain data for Self-242168</t>
-  </si>
-  <si>
     <t>Mr. Nishith Ramesh Gandhi</t>
   </si>
   <si>
@@ -240,9 +237,6 @@
   </si>
   <si>
     <t>Trilokchand Barna</t>
-  </si>
-  <si>
-    <t>The Table doesn't contain data for Trilokchand Barna</t>
   </si>
   <si>
     <t>Mr. Ashish Kumar   Sahu</t>
@@ -748,22 +742,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C109" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -792,7 +788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>189872</v>
       </c>
@@ -815,7 +811,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>664309</v>
       </c>
@@ -838,7 +834,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1222399</v>
       </c>
@@ -861,7 +857,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>470792</v>
       </c>
@@ -884,7 +880,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>466562</v>
       </c>
@@ -907,7 +903,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>470581</v>
       </c>
@@ -930,7 +926,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>594942</v>
       </c>
@@ -953,7 +949,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>183459</v>
       </c>
@@ -976,7 +972,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1274279</v>
       </c>
@@ -999,7 +995,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>363001</v>
       </c>
@@ -1022,7 +1018,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>192146</v>
       </c>
@@ -1045,7 +1041,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>588078</v>
       </c>
@@ -1068,7 +1064,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>196457</v>
       </c>
@@ -1091,7 +1087,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>662072</v>
       </c>
@@ -1114,7 +1110,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>242168</v>
       </c>
@@ -1137,7 +1133,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>849233</v>
       </c>
@@ -1160,7 +1156,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>989139</v>
       </c>
@@ -1183,7 +1179,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>725249</v>
       </c>
@@ -1206,7 +1202,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>333973</v>
       </c>
@@ -1229,7 +1225,7 @@
         <v>97.65625</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1275918</v>
       </c>
@@ -1252,7 +1248,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>192146</v>
       </c>
@@ -1275,7 +1271,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>725249</v>
       </c>
@@ -1298,7 +1294,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>183459</v>
       </c>
@@ -1321,9 +1317,9 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>34</v>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>242168</v>
       </c>
       <c r="B25" t="s">
         <v>24</v>
@@ -1331,8 +1327,8 @@
       <c r="C25">
         <v>500</v>
       </c>
-      <c r="D25" t="s">
-        <v>35</v>
+      <c r="D25">
+        <v>3.2</v>
       </c>
       <c r="F25" t="s">
         <v>33</v>
@@ -1344,12 +1340,12 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>187079</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C26">
         <v>200</v>
@@ -1367,12 +1363,12 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>986513</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C27">
         <v>100</v>
@@ -1390,12 +1386,12 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>241280</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C28">
         <v>150</v>
@@ -1404,7 +1400,7 @@
         <v>4.8667999999999996</v>
       </c>
       <c r="F28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G28">
         <v>241280</v>
@@ -1413,12 +1409,12 @@
         <v>4.8667999999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>398055</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C29">
         <v>200</v>
@@ -1427,7 +1423,7 @@
         <v>1.35</v>
       </c>
       <c r="F29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G29">
         <v>241280</v>
@@ -1436,12 +1432,12 @@
         <v>4.8667999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>773267</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C30">
         <v>250</v>
@@ -1450,7 +1446,7 @@
         <v>3.2</v>
       </c>
       <c r="F30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G30">
         <v>241280</v>
@@ -1459,12 +1455,12 @@
         <v>4.8667999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1062403</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C31">
         <v>300</v>
@@ -1473,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G31">
         <v>241280</v>
@@ -1482,12 +1478,12 @@
         <v>4.8667999999999996</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1275918</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C32">
         <v>100</v>
@@ -1496,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G32">
         <v>241280</v>
@@ -1505,12 +1501,12 @@
         <v>4.8667999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>587873</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C33">
         <v>200</v>
@@ -1519,7 +1515,7 @@
         <v>0.05</v>
       </c>
       <c r="F33" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G33">
         <v>1274279</v>
@@ -1528,12 +1524,12 @@
         <v>0.16875000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>329126</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C34">
         <v>200</v>
@@ -1542,7 +1538,7 @@
         <v>1.9652000000000001</v>
       </c>
       <c r="F34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G34">
         <v>1274279</v>
@@ -1551,12 +1547,12 @@
         <v>0.16875000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>662072</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C35">
         <v>200</v>
@@ -1565,7 +1561,7 @@
         <v>2.1437499999999998</v>
       </c>
       <c r="F35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G35">
         <v>1274279</v>
@@ -1574,12 +1570,12 @@
         <v>0.16875000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>662072</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C36">
         <v>200</v>
@@ -1588,7 +1584,7 @@
         <v>2.1437499999999998</v>
       </c>
       <c r="F36" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G36">
         <v>1274279</v>
@@ -1597,12 +1593,12 @@
         <v>0.16875000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1274279</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C37">
         <v>200</v>
@@ -1611,7 +1607,7 @@
         <v>0.16875000000000001</v>
       </c>
       <c r="F37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G37">
         <v>1274279</v>
@@ -1620,12 +1616,12 @@
         <v>0.16875000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>594942</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C38">
         <v>600</v>
@@ -1643,12 +1639,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>596191</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C39">
         <v>200</v>
@@ -1666,12 +1662,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>661824</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C40">
         <v>200</v>
@@ -1689,12 +1685,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>242146</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C41">
         <v>200</v>
@@ -1703,7 +1699,7 @@
         <v>0.78125</v>
       </c>
       <c r="F41" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G41">
         <v>1034820</v>
@@ -1712,12 +1708,12 @@
         <v>29.635200000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1034820</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C42">
         <v>300</v>
@@ -1726,7 +1722,7 @@
         <v>29.635200000000001</v>
       </c>
       <c r="F42" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G42">
         <v>1034820</v>
@@ -1735,7 +1731,7 @@
         <v>29.635200000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>594942</v>
       </c>
@@ -1749,7 +1745,7 @@
         <v>0.4</v>
       </c>
       <c r="F43" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G43">
         <v>1034820</v>
@@ -1758,12 +1754,12 @@
         <v>29.635200000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>202609</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C44">
         <v>100</v>
@@ -1772,7 +1768,7 @@
         <v>2.1437499999999998</v>
       </c>
       <c r="F44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G44">
         <v>1034820</v>
@@ -1781,12 +1777,12 @@
         <v>29.635200000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1078244</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C45">
         <v>100</v>
@@ -1795,7 +1791,7 @@
         <v>2.1437499999999998</v>
       </c>
       <c r="F45" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G45">
         <v>1034820</v>
@@ -1804,12 +1800,12 @@
         <v>29.635200000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1210517</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C46">
         <v>100</v>
@@ -1818,7 +1814,7 @@
         <v>0.16875000000000001</v>
       </c>
       <c r="F46" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G46">
         <v>1034820</v>
@@ -1827,12 +1823,12 @@
         <v>29.635200000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>598098</v>
       </c>
       <c r="B47" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C47">
         <v>200</v>
@@ -1841,7 +1837,7 @@
         <v>0.4</v>
       </c>
       <c r="F47" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G47">
         <v>598098</v>
@@ -1850,12 +1846,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>596191</v>
       </c>
       <c r="B48" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C48">
         <v>200</v>
@@ -1864,7 +1860,7 @@
         <v>0.98414999999999997</v>
       </c>
       <c r="F48" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G48">
         <v>598098</v>
@@ -1873,7 +1869,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>594942</v>
       </c>
@@ -1887,7 +1883,7 @@
         <v>0.4</v>
       </c>
       <c r="F49" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G49">
         <v>598098</v>
@@ -1896,12 +1892,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>242146</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C50">
         <v>200</v>
@@ -1910,7 +1906,7 @@
         <v>0.78125</v>
       </c>
       <c r="F50" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G50">
         <v>598098</v>
@@ -1919,12 +1915,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>343487</v>
       </c>
       <c r="B51" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C51">
         <v>200</v>
@@ -1933,7 +1929,7 @@
         <v>30</v>
       </c>
       <c r="F51" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G51">
         <v>598098</v>
@@ -1942,12 +1938,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>555704</v>
       </c>
       <c r="B52" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C52">
         <v>400</v>
@@ -1956,7 +1952,7 @@
         <v>0.4</v>
       </c>
       <c r="F52" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G52">
         <v>1210517</v>
@@ -1965,12 +1961,12 @@
         <v>0.16875000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1210517</v>
       </c>
       <c r="B53" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C53">
         <v>400</v>
@@ -1979,7 +1975,7 @@
         <v>0.16875000000000001</v>
       </c>
       <c r="F53" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G53">
         <v>1210517</v>
@@ -1988,7 +1984,7 @@
         <v>0.16875000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>594942</v>
       </c>
@@ -2002,7 +1998,7 @@
         <v>0.4</v>
       </c>
       <c r="F54" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G54">
         <v>1210517</v>
@@ -2011,12 +2007,12 @@
         <v>0.16875000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>558009</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C55">
         <v>100</v>
@@ -2025,7 +2021,7 @@
         <v>0.69120000000000004</v>
       </c>
       <c r="F55" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G55">
         <v>1210517</v>
@@ -2034,12 +2030,12 @@
         <v>0.16875000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>799238</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C56">
         <v>500</v>
@@ -2048,7 +2044,7 @@
         <v>0.16875000000000001</v>
       </c>
       <c r="F56" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G56">
         <v>1060648</v>
@@ -2057,12 +2053,12 @@
         <v>12.50235</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1263467</v>
       </c>
       <c r="B57" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C57">
         <v>500</v>
@@ -2071,7 +2067,7 @@
         <v>32.925150000000002</v>
       </c>
       <c r="F57" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G57">
         <v>1060648</v>
@@ -2080,12 +2076,12 @@
         <v>12.50235</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>598098</v>
       </c>
       <c r="B58" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C58">
         <v>200</v>
@@ -2094,7 +2090,7 @@
         <v>0.4</v>
       </c>
       <c r="F58" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G58">
         <v>596191</v>
@@ -2103,12 +2099,12 @@
         <v>0.98414999999999997</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>596191</v>
       </c>
       <c r="B59" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C59">
         <v>200</v>
@@ -2117,7 +2113,7 @@
         <v>0.98414999999999997</v>
       </c>
       <c r="F59" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G59">
         <v>596191</v>
@@ -2126,7 +2122,7 @@
         <v>0.98414999999999997</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>594942</v>
       </c>
@@ -2140,7 +2136,7 @@
         <v>0.4</v>
       </c>
       <c r="F60" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G60">
         <v>596191</v>
@@ -2149,12 +2145,12 @@
         <v>0.98414999999999997</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>242146</v>
       </c>
       <c r="B61" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C61">
         <v>200</v>
@@ -2163,7 +2159,7 @@
         <v>0.78125</v>
       </c>
       <c r="F61" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G61">
         <v>596191</v>
@@ -2172,12 +2168,12 @@
         <v>0.98414999999999997</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>343487</v>
       </c>
       <c r="B62" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C62">
         <v>200</v>
@@ -2186,7 +2182,7 @@
         <v>30</v>
       </c>
       <c r="F62" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G62">
         <v>596191</v>
@@ -2195,12 +2191,12 @@
         <v>0.98414999999999997</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1263467</v>
       </c>
       <c r="B63" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C63">
         <v>500</v>
@@ -2209,7 +2205,7 @@
         <v>32.925150000000002</v>
       </c>
       <c r="F63" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G63">
         <v>799238</v>
@@ -2218,12 +2214,12 @@
         <v>0.16875000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1060648</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C64">
         <v>500</v>
@@ -2232,7 +2228,7 @@
         <v>12.50235</v>
       </c>
       <c r="F64" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G64">
         <v>799238</v>
@@ -2241,12 +2237,12 @@
         <v>0.16875000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>382819</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C65">
         <v>1000</v>
@@ -2254,22 +2250,22 @@
       <c r="D65">
         <v>6.25</v>
       </c>
-      <c r="F65">
+      <c r="F65" t="s">
+        <v>69</v>
+      </c>
+      <c r="G65">
         <v>382819</v>
       </c>
-      <c r="G65" t="s">
-        <v>71</v>
-      </c>
-      <c r="H65" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H65">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1210517</v>
       </c>
       <c r="B66" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C66">
         <v>300</v>
@@ -2278,7 +2274,7 @@
         <v>0.16875000000000001</v>
       </c>
       <c r="F66" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G66">
         <v>555704</v>
@@ -2287,12 +2283,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>555704</v>
       </c>
       <c r="B67" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C67">
         <v>300</v>
@@ -2301,7 +2297,7 @@
         <v>0.4</v>
       </c>
       <c r="F67" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G67">
         <v>555704</v>
@@ -2310,12 +2306,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>558009</v>
       </c>
       <c r="B68" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C68">
         <v>50</v>
@@ -2324,7 +2320,7 @@
         <v>0.69120000000000004</v>
       </c>
       <c r="F68" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G68">
         <v>555704</v>
@@ -2333,7 +2329,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>664309</v>
       </c>
@@ -2347,7 +2343,7 @@
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="F69" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G69">
         <v>555704</v>
@@ -2356,7 +2352,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1274279</v>
       </c>
@@ -2370,7 +2366,7 @@
         <v>0.16875000000000001</v>
       </c>
       <c r="F70" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G70">
         <v>555704</v>
@@ -2379,12 +2375,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>397341</v>
       </c>
       <c r="B71" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C71">
         <v>100</v>
@@ -2393,7 +2389,7 @@
         <v>0.69120000000000004</v>
       </c>
       <c r="F71" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G71">
         <v>555704</v>
@@ -2402,7 +2398,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>588078</v>
       </c>
@@ -2416,7 +2412,7 @@
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="F72" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G72">
         <v>555704</v>
@@ -2425,12 +2421,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>669418</v>
       </c>
       <c r="B73" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C73">
         <v>400</v>
@@ -2439,7 +2435,7 @@
         <v>30.706250000000001</v>
       </c>
       <c r="F73" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G73">
         <v>669418</v>
@@ -2448,12 +2444,12 @@
         <v>30.706250000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1403167</v>
       </c>
       <c r="B74" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C74">
         <v>150</v>
@@ -2462,7 +2458,7 @@
         <v>31.802800000000001</v>
       </c>
       <c r="F74" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G74">
         <v>669418</v>
@@ -2471,12 +2467,12 @@
         <v>30.706250000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>140816</v>
       </c>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C75">
         <v>150</v>
@@ -2485,7 +2481,7 @@
         <v>16.425450000000001</v>
       </c>
       <c r="F75" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G75">
         <v>669418</v>
@@ -2494,12 +2490,12 @@
         <v>30.706250000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>329126</v>
       </c>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C76">
         <v>100</v>
@@ -2508,7 +2504,7 @@
         <v>1.9652000000000001</v>
       </c>
       <c r="F76" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G76">
         <v>669418</v>
@@ -2517,12 +2513,12 @@
         <v>30.706250000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>510469</v>
       </c>
       <c r="B77" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C77">
         <v>100</v>
@@ -2531,7 +2527,7 @@
         <v>2.5326499999999998</v>
       </c>
       <c r="F77" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G77">
         <v>669418</v>
@@ -2540,7 +2536,7 @@
         <v>30.706250000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>189872</v>
       </c>
@@ -2554,7 +2550,7 @@
         <v>0</v>
       </c>
       <c r="F78" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G78">
         <v>669418</v>
@@ -2563,12 +2559,12 @@
         <v>30.706250000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>854532</v>
       </c>
       <c r="B79" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C79">
         <v>50</v>
@@ -2577,7 +2573,7 @@
         <v>0.78125</v>
       </c>
       <c r="F79" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G79">
         <v>669418</v>
@@ -2586,12 +2582,12 @@
         <v>30.706250000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1271241</v>
       </c>
       <c r="B80" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C80">
         <v>100</v>
@@ -2600,7 +2596,7 @@
         <v>241.34045</v>
       </c>
       <c r="F80" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G80">
         <v>465114</v>
@@ -2609,12 +2605,12 @@
         <v>7.8731999999999998</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>341538</v>
       </c>
       <c r="B81" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C81">
         <v>100</v>
@@ -2623,7 +2619,7 @@
         <v>88.578050000000005</v>
       </c>
       <c r="F81" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G81">
         <v>465114</v>
@@ -2632,12 +2628,12 @@
         <v>7.8731999999999998</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>730067</v>
       </c>
       <c r="B82" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C82">
         <v>100</v>
@@ -2646,7 +2642,7 @@
         <v>48.514949999999999</v>
       </c>
       <c r="F82" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G82">
         <v>465114</v>
@@ -2655,12 +2651,12 @@
         <v>7.8731999999999998</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1263467</v>
       </c>
       <c r="B83" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C83">
         <v>100</v>
@@ -2669,7 +2665,7 @@
         <v>32.925150000000002</v>
       </c>
       <c r="F83" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G83">
         <v>465114</v>
@@ -2678,12 +2674,12 @@
         <v>7.8731999999999998</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1202864</v>
       </c>
       <c r="B84" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C84">
         <v>100</v>
@@ -2692,7 +2688,7 @@
         <v>29.635200000000001</v>
       </c>
       <c r="F84" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G84">
         <v>465114</v>
@@ -2701,12 +2697,12 @@
         <v>7.8731999999999998</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>977151</v>
       </c>
       <c r="B85" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C85">
         <v>100</v>
@@ -2715,7 +2711,7 @@
         <v>9.2596500000000006</v>
       </c>
       <c r="F85" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G85">
         <v>465114</v>
@@ -2724,12 +2720,12 @@
         <v>7.8731999999999998</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>205581</v>
       </c>
       <c r="B86" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C86">
         <v>100</v>
@@ -2738,7 +2734,7 @@
         <v>0.16875000000000001</v>
       </c>
       <c r="F86" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G86">
         <v>465114</v>
@@ -2747,12 +2743,12 @@
         <v>7.8731999999999998</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>231045</v>
       </c>
       <c r="B87" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C87">
         <v>200</v>
@@ -2761,7 +2757,7 @@
         <v>0.4</v>
       </c>
       <c r="F87" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G87">
         <v>231045</v>
@@ -2770,12 +2766,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1077053</v>
       </c>
       <c r="B88" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C88">
         <v>200</v>
@@ -2784,7 +2780,7 @@
         <v>0.05</v>
       </c>
       <c r="F88" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G88">
         <v>231045</v>
@@ -2793,12 +2789,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>764679</v>
       </c>
       <c r="B89" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C89">
         <v>200</v>
@@ -2807,7 +2803,7 @@
         <v>32.925150000000002</v>
       </c>
       <c r="F89" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G89">
         <v>231045</v>
@@ -2816,12 +2812,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>684328</v>
       </c>
       <c r="B90" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C90">
         <v>100</v>
@@ -2830,7 +2826,7 @@
         <v>51.515050000000002</v>
       </c>
       <c r="F90" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G90">
         <v>231045</v>
@@ -2839,12 +2835,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>242989</v>
       </c>
       <c r="B91" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C91">
         <v>300</v>
@@ -2853,7 +2849,7 @@
         <v>30</v>
       </c>
       <c r="F91" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G91">
         <v>231045</v>
@@ -2862,12 +2858,12 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1275918</v>
       </c>
       <c r="B92" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C92">
         <v>100</v>
@@ -2876,7 +2872,7 @@
         <v>0</v>
       </c>
       <c r="F92" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G92">
         <v>242989</v>
@@ -2885,12 +2881,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>189872</v>
       </c>
       <c r="B93" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C93">
         <v>100</v>
@@ -2899,7 +2895,7 @@
         <v>0</v>
       </c>
       <c r="F93" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G93">
         <v>242989</v>
@@ -2908,12 +2904,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>186196</v>
       </c>
       <c r="B94" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C94">
         <v>100</v>
@@ -2922,7 +2918,7 @@
         <v>19.450849999999999</v>
       </c>
       <c r="F94" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G94">
         <v>242989</v>
@@ -2931,12 +2927,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1202864</v>
       </c>
       <c r="B95" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C95">
         <v>100</v>
@@ -2945,7 +2941,7 @@
         <v>29.635200000000001</v>
       </c>
       <c r="F95" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G95">
         <v>242989</v>
@@ -2954,12 +2950,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>558009</v>
       </c>
       <c r="B96" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C96">
         <v>100</v>
@@ -2968,7 +2964,7 @@
         <v>0.69120000000000004</v>
       </c>
       <c r="F96" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G96">
         <v>242989</v>
@@ -2977,12 +2973,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1264140</v>
       </c>
       <c r="B97" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C97">
         <v>100</v>
@@ -2991,7 +2987,7 @@
         <v>0.4</v>
       </c>
       <c r="F97" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G97">
         <v>242989</v>
@@ -3000,12 +2996,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1062403</v>
       </c>
       <c r="B98" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C98">
         <v>100</v>
@@ -3014,7 +3010,7 @@
         <v>0</v>
       </c>
       <c r="F98" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G98">
         <v>242989</v>
@@ -3023,12 +3019,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>363001</v>
       </c>
       <c r="B99" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C99">
         <v>100</v>
@@ -3037,7 +3033,7 @@
         <v>0.05</v>
       </c>
       <c r="F99" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G99">
         <v>242989</v>
@@ -3046,12 +3042,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>183459</v>
       </c>
       <c r="B100" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C100">
         <v>100</v>
@@ -3060,7 +3056,7 @@
         <v>0.4</v>
       </c>
       <c r="F100" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G100">
         <v>242989</v>
@@ -3069,12 +3065,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>242146</v>
       </c>
       <c r="B101" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C101">
         <v>100</v>
@@ -3083,7 +3079,7 @@
         <v>0.78125</v>
       </c>
       <c r="F101" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G101">
         <v>242989</v>
@@ -3092,12 +3088,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>849233</v>
       </c>
       <c r="B102" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C102">
         <v>200</v>
@@ -3115,7 +3111,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>183459</v>
       </c>
@@ -3138,12 +3134,12 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>986513</v>
       </c>
       <c r="B104" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C104">
         <v>200</v>
@@ -3161,7 +3157,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>664309</v>
       </c>
@@ -3184,12 +3180,12 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>799238</v>
       </c>
       <c r="B106" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C106">
         <v>500</v>
@@ -3198,7 +3194,7 @@
         <v>0.16875000000000001</v>
       </c>
       <c r="F106" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G106">
         <v>1263467</v>
@@ -3207,12 +3203,12 @@
         <v>32.925150000000002</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>1060648</v>
       </c>
       <c r="B107" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C107">
         <v>500</v>
@@ -3221,7 +3217,7 @@
         <v>12.50235</v>
       </c>
       <c r="F107" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G107">
         <v>1263467</v>
@@ -3230,12 +3226,12 @@
         <v>32.925150000000002</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>189872</v>
       </c>
       <c r="B108" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C108">
         <v>200</v>
@@ -3244,10 +3240,10 @@
         <v>0</v>
       </c>
       <c r="H108" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>183459</v>
       </c>
@@ -3261,15 +3257,15 @@
         <v>0.4</v>
       </c>
       <c r="H109" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>335878</v>
       </c>
       <c r="B110" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C110">
         <v>200</v>
@@ -3278,10 +3274,10 @@
         <v>30</v>
       </c>
       <c r="H110" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>192146</v>
       </c>
@@ -3295,10 +3291,10 @@
         <v>0.05</v>
       </c>
       <c r="H111" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>470581</v>
       </c>
@@ -3312,15 +3308,15 @@
         <v>35.248449999999998</v>
       </c>
       <c r="H112" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>1034820</v>
       </c>
       <c r="B113" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C113">
         <v>300</v>
@@ -3329,7 +3325,7 @@
         <v>29.635200000000001</v>
       </c>
       <c r="F113" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G113">
         <v>1078244</v>
@@ -3338,12 +3334,12 @@
         <v>2.1437499999999998</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>684328</v>
       </c>
       <c r="B114" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C114">
         <v>300</v>
@@ -3352,7 +3348,7 @@
         <v>51.515050000000002</v>
       </c>
       <c r="F114" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G114">
         <v>1078244</v>
@@ -3361,12 +3357,12 @@
         <v>2.1437499999999998</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>854532</v>
       </c>
       <c r="B115" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C115">
         <v>400</v>
@@ -3375,7 +3371,7 @@
         <v>0.78125</v>
       </c>
       <c r="F115" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G115">
         <v>1078244</v>
@@ -3384,12 +3380,12 @@
         <v>2.1437499999999998</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>598098</v>
       </c>
       <c r="B116" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C116">
         <v>100</v>
@@ -3398,7 +3394,7 @@
         <v>0.4</v>
       </c>
       <c r="F116" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G116">
         <v>202609</v>
@@ -3407,12 +3403,12 @@
         <v>2.1437499999999998</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>594942</v>
       </c>
       <c r="B117" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C117">
         <v>100</v>
@@ -3421,7 +3417,7 @@
         <v>0.4</v>
       </c>
       <c r="F117" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G117">
         <v>202609</v>
@@ -3430,12 +3426,12 @@
         <v>2.1437499999999998</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>596191</v>
       </c>
       <c r="B118" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C118">
         <v>100</v>
@@ -3444,7 +3440,7 @@
         <v>0.98414999999999997</v>
       </c>
       <c r="F118" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G118">
         <v>202609</v>
@@ -3453,12 +3449,12 @@
         <v>2.1437499999999998</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>242146</v>
       </c>
       <c r="B119" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C119">
         <v>100</v>
@@ -3467,7 +3463,7 @@
         <v>0.78125</v>
       </c>
       <c r="F119" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G119">
         <v>202609</v>
@@ -3476,12 +3472,12 @@
         <v>2.1437499999999998</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>1210517</v>
       </c>
       <c r="B120" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C120">
         <v>100</v>
@@ -3490,7 +3486,7 @@
         <v>0.16875000000000001</v>
       </c>
       <c r="F120" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G120">
         <v>202609</v>
@@ -3499,12 +3495,12 @@
         <v>2.1437499999999998</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>202609</v>
       </c>
       <c r="B121" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C121">
         <v>500</v>
@@ -3513,7 +3509,7 @@
         <v>2.1437499999999998</v>
       </c>
       <c r="F121" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G121">
         <v>202609</v>
@@ -3522,7 +3518,7 @@
         <v>2.1437499999999998</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>363001</v>
       </c>
@@ -3536,7 +3532,7 @@
         <v>0.05</v>
       </c>
       <c r="F122" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G122">
         <v>242146</v>
@@ -3545,12 +3541,12 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>598098</v>
       </c>
       <c r="B123" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C123">
         <v>100</v>
@@ -3559,7 +3555,7 @@
         <v>0.4</v>
       </c>
       <c r="F123" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G123">
         <v>242146</v>
@@ -3568,12 +3564,12 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>202609</v>
       </c>
       <c r="B124" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C124">
         <v>100</v>
@@ -3582,7 +3578,7 @@
         <v>2.1437499999999998</v>
       </c>
       <c r="F124" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G124">
         <v>242146</v>
@@ -3591,12 +3587,12 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>1034820</v>
       </c>
       <c r="B125" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C125">
         <v>100</v>
@@ -3605,7 +3601,7 @@
         <v>29.635200000000001</v>
       </c>
       <c r="F125" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G125">
         <v>242146</v>
@@ -3614,12 +3610,12 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>558009</v>
       </c>
       <c r="B126" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C126">
         <v>100</v>
@@ -3628,7 +3624,7 @@
         <v>0.69120000000000004</v>
       </c>
       <c r="F126" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G126">
         <v>242146</v>
@@ -3637,12 +3633,12 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>596191</v>
       </c>
       <c r="B127" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C127">
         <v>100</v>
@@ -3651,7 +3647,7 @@
         <v>0.98414999999999997</v>
       </c>
       <c r="F127" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G127">
         <v>242146</v>
@@ -3660,12 +3656,12 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>178120</v>
       </c>
       <c r="B128" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C128">
         <v>100</v>
@@ -3674,7 +3670,7 @@
         <v>30</v>
       </c>
       <c r="F128" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G128">
         <v>242146</v>
@@ -3683,12 +3679,12 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>1210517</v>
       </c>
       <c r="B129" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C129">
         <v>100</v>
@@ -3697,7 +3693,7 @@
         <v>0.16875000000000001</v>
       </c>
       <c r="F129" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G129">
         <v>242146</v>
@@ -3706,12 +3702,12 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>555704</v>
       </c>
       <c r="B130" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C130">
         <v>100</v>
@@ -3720,7 +3716,7 @@
         <v>0.4</v>
       </c>
       <c r="F130" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G130">
         <v>242146</v>
@@ -3729,7 +3725,7 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>594942</v>
       </c>
@@ -3743,7 +3739,7 @@
         <v>0.4</v>
       </c>
       <c r="F131" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G131">
         <v>242146</v>
@@ -3752,12 +3748,12 @@
         <v>0.78125</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>1034820</v>
       </c>
       <c r="B132" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C132">
         <v>300</v>
@@ -3766,7 +3762,7 @@
         <v>29.635200000000001</v>
       </c>
       <c r="F132" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G132">
         <v>662072</v>
@@ -3775,12 +3771,12 @@
         <v>2.1437499999999998</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>684328</v>
       </c>
       <c r="B133" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C133">
         <v>300</v>
@@ -3789,7 +3785,7 @@
         <v>51.515050000000002</v>
       </c>
       <c r="F133" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G133">
         <v>662072</v>
@@ -3798,12 +3794,12 @@
         <v>2.1437499999999998</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>854532</v>
       </c>
       <c r="B134" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C134">
         <v>400</v>
@@ -3812,7 +3808,7 @@
         <v>0.78125</v>
       </c>
       <c r="F134" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G134">
         <v>662072</v>
@@ -3821,12 +3817,12 @@
         <v>2.1437499999999998</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>1403167</v>
       </c>
       <c r="B135" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C135">
         <v>200</v>
@@ -3835,7 +3831,7 @@
         <v>31.802800000000001</v>
       </c>
       <c r="F135" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G135">
         <v>1403167</v>
@@ -3844,12 +3840,12 @@
         <v>31.802800000000001</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>510469</v>
       </c>
       <c r="B136" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C136">
         <v>500</v>
@@ -3858,7 +3854,7 @@
         <v>2.5326499999999998</v>
       </c>
       <c r="F136" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G136">
         <v>1403167</v>
@@ -3867,12 +3863,12 @@
         <v>31.802800000000001</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>669418</v>
       </c>
       <c r="B137" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C137">
         <v>100</v>
@@ -3881,7 +3877,7 @@
         <v>30.706250000000001</v>
       </c>
       <c r="F137" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G137">
         <v>1403167</v>
@@ -3890,12 +3886,12 @@
         <v>31.802800000000001</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>140816</v>
       </c>
       <c r="B138" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C138">
         <v>200</v>
@@ -3904,7 +3900,7 @@
         <v>16.425450000000001</v>
       </c>
       <c r="F138" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G138">
         <v>1403167</v>

</xml_diff>